<commit_message>
changed readme and excel
</commit_message>
<xml_diff>
--- a/datas/塩分濃度.xlsx
+++ b/datas/塩分濃度.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kosenjp-my.sharepoint.com/personal/ic191209_edu_okinawa-ct_ac_jp/Documents/5年/卒研/実験データちゃんたち/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{D874DF49-B940-4F9E-BE25-81EE9C7C4164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{200CDD66-7E9F-4BC0-80C9-7B79F6D62412}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{D874DF49-B940-4F9E-BE25-81EE9C7C4164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D00A8AE7-B7AD-4C86-A1ED-ECAFC0A0EC4F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="11" xr2:uid="{9BBC037C-80C6-4454-89DC-D4BC2DF4D696}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9BBC037C-80C6-4454-89DC-D4BC2DF4D696}"/>
   </bookViews>
   <sheets>
-    <sheet name="template" sheetId="3" r:id="rId1"/>
-    <sheet name="各実験時間" sheetId="8" r:id="rId2"/>
-    <sheet name="1_15" sheetId="1" r:id="rId3"/>
-    <sheet name="1_16" sheetId="4" r:id="rId4"/>
-    <sheet name="1_17" sheetId="6" r:id="rId5"/>
-    <sheet name="1_18" sheetId="7" r:id="rId6"/>
-    <sheet name="1_19" sheetId="9" r:id="rId7"/>
-    <sheet name="1_22" sheetId="12" r:id="rId8"/>
-    <sheet name="1_24" sheetId="13" r:id="rId9"/>
-    <sheet name="1_29" sheetId="15" r:id="rId10"/>
-    <sheet name="1_30" sheetId="17" r:id="rId11"/>
-    <sheet name="1_31" sheetId="19" r:id="rId12"/>
+    <sheet name="README" sheetId="22" r:id="rId1"/>
+    <sheet name="template" sheetId="3" r:id="rId2"/>
+    <sheet name="各実験時間" sheetId="8" r:id="rId3"/>
+    <sheet name="1_15" sheetId="1" r:id="rId4"/>
+    <sheet name="1_16" sheetId="4" r:id="rId5"/>
+    <sheet name="1_17" sheetId="6" r:id="rId6"/>
+    <sheet name="1_18" sheetId="7" r:id="rId7"/>
+    <sheet name="1_19" sheetId="9" r:id="rId8"/>
+    <sheet name="1_22" sheetId="12" r:id="rId9"/>
+    <sheet name="1_24" sheetId="13" r:id="rId10"/>
+    <sheet name="1_29" sheetId="15" r:id="rId11"/>
+    <sheet name="1_30" sheetId="17" r:id="rId12"/>
+    <sheet name="1_31" sheetId="19" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="47">
   <si>
     <t>時間</t>
     <rPh sb="0" eb="2">
@@ -557,6 +558,55 @@
     </rPh>
     <rPh sb="6" eb="7">
       <t>ナシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここにデータを入力</t>
+    <rPh sb="7" eb="9">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※使い方</t>
+    <rPh sb="1" eb="2">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実験前…塩の重量を記録しましょう
+実験中...時間とその時の塩分濃度を記録しましょう</t>
+    <rPh sb="0" eb="3">
+      <t>ジッケンマエ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>シオ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジュウリョウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>キロク</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>ジッケンチュウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="30" eb="34">
+      <t>エンブンノウド</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>キロク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -611,7 +661,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -957,13 +1007,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1045,6 +1183,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1060,6 +1222,257 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8458EC2-A876-16FC-FF2D-AE7446C4C490}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="323850" y="889000"/>
+          <a:ext cx="10712450" cy="527050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1873250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66893C76-5A91-4399-927E-053DD41BC7CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2235200" y="431800"/>
+          <a:ext cx="863600" cy="292100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直線矢印コネクタ 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDFED96F-430F-6778-FBDC-D259C495B813}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="3" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3098800" y="577850"/>
+          <a:ext cx="609600" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直線矢印コネクタ 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A7EBE5E-C3CB-496B-B21F-92E4B8628D61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5022850" y="577850"/>
+          <a:ext cx="412750" cy="260350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1358,11 +1771,666 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B6C67-6B2F-472E-B937-AE06E8D6FB89}">
-  <dimension ref="B1:O18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7362A03D-3C95-4CB1-834E-C516ACAA2D9B}">
+  <dimension ref="B1:P19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1">
+        <f>156/3</f>
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="I2" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="31"/>
+    </row>
+    <row r="3" spans="2:16" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>140</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="34"/>
+    </row>
+    <row r="4" spans="2:16" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="5" spans="2:16" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.37708333333333338</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.66388888888888886</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.78125</v>
+      </c>
+      <c r="G5" s="17">
+        <v>1.3576388888888891</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="19"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6.85</v>
+      </c>
+      <c r="G6" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5">
+        <f>$C$3*((100/C6)-1)</f>
+        <v>3041.8181818181815</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" ref="D7:O7" si="0">$C$3*((100/D6)-1)</f>
+        <v>2838.7234042553191</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>2193.3333333333335</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>1903.7956204379561</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>1365.3763440860214</v>
+      </c>
+      <c r="H7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <f>C7-D7</f>
+        <v>203.09477756286242</v>
+      </c>
+      <c r="E8" s="1">
+        <f>D7-E7</f>
+        <v>645.39007092198563</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E7-F7</f>
+        <v>289.53771289537735</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:O8" si="1">F7-G7</f>
+        <v>538.41927635193474</v>
+      </c>
+      <c r="H8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="20">
+        <f>(D5-C5)*24</f>
+        <v>3.5833333333333326</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" ref="E9:O9" si="2">(E5-D5)*24</f>
+        <v>3.2999999999999989</v>
+      </c>
+      <c r="F9" s="20">
+        <f t="shared" si="2"/>
+        <v>2.8166666666666673</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="2"/>
+        <v>13.833333333333337</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="2"/>
+        <v>-32.583333333333336</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8">
+        <f>D8/D9</f>
+        <v>56.677612343124409</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10:O10" si="3">E8/E9</f>
+        <v>195.57274876423813</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="3"/>
+        <v>102.79445428238247</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="3"/>
+        <v>38.921875398935029</v>
+      </c>
+      <c r="H10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" s="23" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="13" spans="2:16" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.37708333333333338</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.66388888888888886</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.78125</v>
+      </c>
+      <c r="G13" s="17">
+        <v>1.3576388888888891</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="19"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="G14" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5">
+        <f>$C$3*((100/C14)-1)</f>
+        <v>2838.7234042553191</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" ref="D15:O15" si="4">$C$3*((100/D14)-1)</f>
+        <v>2903.4782608695655</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="4"/>
+        <v>2838.7234042553191</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="4"/>
+        <v>2776.666666666667</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="4"/>
+        <v>2776.666666666667</v>
+      </c>
+      <c r="H15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <f>C15-D15</f>
+        <v>-64.754856614246364</v>
+      </c>
+      <c r="E16" s="1">
+        <f>D15-E15</f>
+        <v>64.754856614246364</v>
+      </c>
+      <c r="F16" s="1">
+        <f>E15-F15</f>
+        <v>62.05673758865214</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:O16" si="5">F15-G15</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="6" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="20">
+        <f>(D13-C13)*24</f>
+        <v>3.5833333333333326</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" ref="E17:O17" si="6">(E13-D13)*24</f>
+        <v>3.2999999999999989</v>
+      </c>
+      <c r="F17" s="20">
+        <f t="shared" si="6"/>
+        <v>2.8166666666666673</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" si="6"/>
+        <v>13.833333333333337</v>
+      </c>
+      <c r="H17" s="20">
+        <f t="shared" si="6"/>
+        <v>-32.583333333333336</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8">
+        <f>D16/D17</f>
+        <v>-18.071122776068755</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" ref="E18:O18" si="7">E16/E17</f>
+        <v>19.622683822498903</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="7"/>
+        <v>22.031977842125016</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="8" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="23" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J2:P3"/>
+    <mergeCell ref="I2:I3"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9329DD8B-65E1-47BD-9476-D29FF2DD3E97}">
+  <dimension ref="B1:O19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1374,7 +2442,17 @@
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1">
+        <f>156/3</f>
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.55000000000000004">
@@ -1396,11 +2474,21 @@
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
+      <c r="C5" s="18">
+        <v>0.37708333333333338</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.66388888888888886</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.78125</v>
+      </c>
+      <c r="G5" s="17">
+        <v>1.3576388888888891</v>
+      </c>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
@@ -1414,11 +2502,21 @@
       <c r="B6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="C6" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6.85</v>
+      </c>
+      <c r="G6" s="3">
+        <v>9.3000000000000007</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1432,25 +2530,25 @@
       <c r="B7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="e">
+      <c r="C7" s="5">
         <f>$C$3*((100/C6)-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D7" s="9" t="e">
+        <v>3041.8181818181815</v>
+      </c>
+      <c r="D7" s="9">
         <f t="shared" ref="D7:O7" si="0">$C$3*((100/D6)-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2838.7234042553191</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>2193.3333333333335</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>1903.7956204379561</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>1365.3763440860214</v>
       </c>
       <c r="H7" s="9" t="e">
         <f t="shared" si="0"/>
@@ -1492,21 +2590,21 @@
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="1" t="e">
+      <c r="D8" s="1">
         <f>C7-D7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E8" s="1" t="e">
+        <v>203.09477756286242</v>
+      </c>
+      <c r="E8" s="1">
         <f>D7-E7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="1" t="e">
+        <v>645.39007092198563</v>
+      </c>
+      <c r="F8" s="1">
         <f>E7-F7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" s="1" t="e">
+        <v>289.53771289537735</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" ref="G8:O8" si="1">F7-G7</f>
-        <v>#DIV/0!</v>
+        <v>538.41927635193474</v>
       </c>
       <c r="H8" s="1" t="e">
         <f t="shared" si="1"/>
@@ -1550,23 +2648,23 @@
       </c>
       <c r="D9" s="20">
         <f>(D5-C5)*24</f>
-        <v>0</v>
+        <v>3.5833333333333326</v>
       </c>
       <c r="E9" s="20">
         <f t="shared" ref="E9:O9" si="2">(E5-D5)*24</f>
-        <v>0</v>
+        <v>3.2999999999999989</v>
       </c>
       <c r="F9" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.8166666666666673</v>
       </c>
       <c r="G9" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13.833333333333337</v>
       </c>
       <c r="H9" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-32.583333333333336</v>
       </c>
       <c r="I9" s="20">
         <f t="shared" si="2"/>
@@ -1604,21 +2702,21 @@
       <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="8" t="e">
+      <c r="D10" s="8">
         <f>D8/D9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" s="8" t="e">
+        <v>56.677612343124409</v>
+      </c>
+      <c r="E10" s="8">
         <f t="shared" ref="E10:O10" si="3">E8/E9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>195.57274876423813</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="3"/>
+        <v>102.79445428238247</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="3"/>
+        <v>38.921875398935029</v>
       </c>
       <c r="H10" s="8" t="e">
         <f t="shared" si="3"/>
@@ -1657,17 +2755,30 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
+      <c r="C11" s="25" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="13" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B13" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="C13" s="18">
+        <v>0.37708333333333338</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="E13" s="17">
+        <v>0.66388888888888886</v>
+      </c>
+      <c r="F13" s="17">
+        <v>0.78125</v>
+      </c>
+      <c r="G13" s="17">
+        <v>1.3576388888888891</v>
+      </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
@@ -1681,11 +2792,21 @@
       <c r="B14" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="C14" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="G14" s="3">
+        <v>4.8</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1699,25 +2820,25 @@
       <c r="B15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="5" t="e">
+      <c r="C15" s="5">
         <f>$C$3*((100/C14)-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" s="9" t="e">
+        <v>2838.7234042553191</v>
+      </c>
+      <c r="D15" s="9">
         <f t="shared" ref="D15:O15" si="4">$C$3*((100/D14)-1)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>2903.4782608695655</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="4"/>
+        <v>2838.7234042553191</v>
+      </c>
+      <c r="F15" s="9">
+        <f t="shared" si="4"/>
+        <v>2776.666666666667</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="4"/>
+        <v>2776.666666666667</v>
       </c>
       <c r="H15" s="9" t="e">
         <f t="shared" si="4"/>
@@ -1759,52 +2880,52 @@
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1" t="e">
+      <c r="D16" s="1">
         <f>C15-D15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="1" t="e">
+        <v>-64.754856614246364</v>
+      </c>
+      <c r="E16" s="1">
         <f>D15-E15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="1" t="e">
+        <v>64.754856614246364</v>
+      </c>
+      <c r="F16" s="1">
         <f>E15-F15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G16" s="1" t="e">
-        <f t="shared" ref="G16" si="5">F15-G15</f>
-        <v>#DIV/0!</v>
+        <v>62.05673758865214</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:O16" si="5">F15-G15</f>
+        <v>0</v>
       </c>
       <c r="H16" s="1" t="e">
-        <f t="shared" ref="H16" si="6">G15-H15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I16" s="1" t="e">
-        <f t="shared" ref="I16" si="7">H15-I15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J16" s="1" t="e">
-        <f t="shared" ref="J16" si="8">I15-J15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="1" t="e">
-        <f t="shared" ref="K16" si="9">J15-K15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="1" t="e">
-        <f t="shared" ref="L16" si="10">K15-L15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="1" t="e">
-        <f t="shared" ref="M16" si="11">L15-M15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N16" s="1" t="e">
-        <f t="shared" ref="N16" si="12">M15-N15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O16" s="6" t="e">
-        <f t="shared" ref="O16" si="13">N15-O15</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1817,50 +2938,50 @@
       </c>
       <c r="D17" s="20">
         <f>(D13-C13)*24</f>
-        <v>0</v>
+        <v>3.5833333333333326</v>
       </c>
       <c r="E17" s="20">
-        <f t="shared" ref="E17" si="14">(E13-D13)*24</f>
-        <v>0</v>
+        <f t="shared" ref="E17:O17" si="6">(E13-D13)*24</f>
+        <v>3.2999999999999989</v>
       </c>
       <c r="F17" s="20">
-        <f t="shared" ref="F17" si="15">(F13-E13)*24</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.8166666666666673</v>
       </c>
       <c r="G17" s="20">
-        <f t="shared" ref="G17" si="16">(G13-F13)*24</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>13.833333333333337</v>
       </c>
       <c r="H17" s="20">
-        <f t="shared" ref="H17" si="17">(H13-G13)*24</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>-32.583333333333336</v>
       </c>
       <c r="I17" s="20">
-        <f t="shared" ref="I17" si="18">(I13-H13)*24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J17" s="20">
-        <f t="shared" ref="J17" si="19">(J13-I13)*24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K17" s="20">
-        <f t="shared" ref="K17" si="20">(K13-J13)*24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L17" s="20">
-        <f t="shared" ref="L17" si="21">(L13-K13)*24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M17" s="20">
-        <f t="shared" ref="M17" si="22">(M13-L13)*24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N17" s="20">
-        <f t="shared" ref="N17" si="23">(N13-M13)*24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O17" s="22">
-        <f t="shared" ref="O17" si="24">(O13-N13)*24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1871,53 +2992,58 @@
       <c r="C18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="8" t="e">
+      <c r="D18" s="8">
         <f>D16/D17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E18" s="8" t="e">
-        <f t="shared" ref="E18:N18" si="25">E16/E17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="8" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="8" t="e">
-        <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>-18.071122776068755</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" ref="E18:O18" si="7">E16/E17</f>
+        <v>19.622683822498903</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="7"/>
+        <v>22.031977842125016</v>
+      </c>
+      <c r="G18" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="H18" s="8" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="I18" s="8" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J18" s="8" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="8" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L18" s="8" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="8" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="8" t="e">
-        <f t="shared" si="25"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O18" s="23" t="e">
-        <f>O16/O17</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" s="25" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1926,7 +3052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3F91E7-CACD-4994-8D9D-2215DABCE853}">
   <dimension ref="A1:O18"/>
   <sheetViews>
@@ -2581,7 +3707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B7D948-C2D2-4573-87F5-186BD1151854}">
   <dimension ref="A1:O18"/>
   <sheetViews>
@@ -3199,12 +4325,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E9D42D-E4CD-4217-83D6-7F3AC0686D21}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3810,6 +4936,575 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632B6C67-6B2F-472E-B937-AE06E8D6FB89}">
+  <dimension ref="B1:O18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="4.75" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="5" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="19"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="e">
+        <f>$C$3*((100/C6)-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D7" s="9" t="e">
+        <f t="shared" ref="D7:O7" si="0">$C$3*((100/D6)-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="e">
+        <f>C7-D7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8" s="1" t="e">
+        <f>D7-E7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="1" t="e">
+        <f>E7-F7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="1" t="e">
+        <f t="shared" ref="G8:O8" si="1">F7-G7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="20">
+        <f>(D5-C5)*24</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" ref="E9:O9" si="2">(E5-D5)*24</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8" t="e">
+        <f>D8/D9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" s="8" t="e">
+        <f t="shared" ref="E10:O10" si="3">E8/E9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" s="23" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="13" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="19"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="e">
+        <f>$C$3*((100/C14)-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="9" t="e">
+        <f t="shared" ref="D15:O15" si="4">$C$3*((100/D14)-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="9" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="e">
+        <f>C15-D15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="1" t="e">
+        <f>D15-E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="1" t="e">
+        <f>E15-F15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="1" t="e">
+        <f t="shared" ref="G16" si="5">F15-G15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="1" t="e">
+        <f t="shared" ref="H16" si="6">G15-H15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="1" t="e">
+        <f t="shared" ref="I16" si="7">H15-I15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="1" t="e">
+        <f t="shared" ref="J16" si="8">I15-J15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="1" t="e">
+        <f t="shared" ref="K16" si="9">J15-K15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" s="1" t="e">
+        <f t="shared" ref="L16" si="10">K15-L15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="1" t="e">
+        <f t="shared" ref="M16" si="11">L15-M15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" s="1" t="e">
+        <f t="shared" ref="N16" si="12">M15-N15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="6" t="e">
+        <f t="shared" ref="O16" si="13">N15-O15</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="20">
+        <f>(D13-C13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" ref="E17" si="14">(E13-D13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="20">
+        <f t="shared" ref="F17" si="15">(F13-E13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" ref="G17" si="16">(G13-F13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="20">
+        <f t="shared" ref="H17" si="17">(H13-G13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" ref="I17" si="18">(I13-H13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="20">
+        <f t="shared" ref="J17" si="19">(J13-I13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="20">
+        <f t="shared" ref="K17" si="20">(K13-J13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" ref="L17" si="21">(L13-K13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="20">
+        <f t="shared" ref="M17" si="22">(M13-L13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="20">
+        <f t="shared" ref="N17" si="23">(N13-M13)*24</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="22">
+        <f t="shared" ref="O17" si="24">(O13-N13)*24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8" t="e">
+        <f>D16/D17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E18" s="8" t="e">
+        <f t="shared" ref="E18:N18" si="25">E16/E17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="8" t="e">
+        <f t="shared" si="25"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="23" t="e">
+        <f>O16/O17</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E142EF28-6E1B-4329-B1C0-4C8D4FE6A963}">
   <dimension ref="B2:Z13"/>
   <sheetViews>
@@ -4012,12 +5707,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDA86B-BFFE-49F4-AB2C-530FA53A231F}">
   <dimension ref="B1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B5" sqref="B5:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -4349,7 +6044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F2793D-AB4E-4795-AF8F-26B3E1911783}">
   <dimension ref="B1:O11"/>
   <sheetViews>
@@ -4705,7 +6400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682A722E-D835-4B71-80E0-54EEE0FEDED7}">
   <dimension ref="A1:O18"/>
   <sheetViews>
@@ -5331,7 +7026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AA2B08-C560-4ACC-8EC5-96D66BF27518}">
   <dimension ref="B1:O18"/>
   <sheetViews>
@@ -5956,11 +7651,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E21F58C-A9D6-48A3-9109-5D4C9AFBABF5}">
   <dimension ref="B1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -6563,7 +8258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28034EC-3E0B-45FF-93A9-B1B4076DE1FB}">
   <dimension ref="B1:O18"/>
   <sheetViews>
@@ -7146,633 +8841,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9329DD8B-65E1-47BD-9476-D29FF2DD3E97}">
-  <dimension ref="B1:O19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="4.75" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1">
-        <f>156/3</f>
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="5" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="18">
-        <v>0.37708333333333338</v>
-      </c>
-      <c r="D5" s="17">
-        <v>0.52638888888888891</v>
-      </c>
-      <c r="E5" s="17">
-        <v>0.66388888888888886</v>
-      </c>
-      <c r="F5" s="17">
-        <v>0.78125</v>
-      </c>
-      <c r="G5" s="17">
-        <v>1.3576388888888891</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="19"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="E6" s="3">
-        <v>6</v>
-      </c>
-      <c r="F6" s="3">
-        <v>6.85</v>
-      </c>
-      <c r="G6" s="3">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5">
-        <f>$C$3*((100/C6)-1)</f>
-        <v>3041.8181818181815</v>
-      </c>
-      <c r="D7" s="9">
-        <f t="shared" ref="D7:O7" si="0">$C$3*((100/D6)-1)</f>
-        <v>2838.7234042553191</v>
-      </c>
-      <c r="E7" s="9">
-        <f t="shared" si="0"/>
-        <v>2193.3333333333335</v>
-      </c>
-      <c r="F7" s="9">
-        <f t="shared" si="0"/>
-        <v>1903.7956204379561</v>
-      </c>
-      <c r="G7" s="9">
-        <f t="shared" si="0"/>
-        <v>1365.3763440860214</v>
-      </c>
-      <c r="H7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" s="9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O7" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <f>C7-D7</f>
-        <v>203.09477756286242</v>
-      </c>
-      <c r="E8" s="1">
-        <f>D7-E7</f>
-        <v>645.39007092198563</v>
-      </c>
-      <c r="F8" s="1">
-        <f>E7-F7</f>
-        <v>289.53771289537735</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" ref="G8:O8" si="1">F7-G7</f>
-        <v>538.41927635193474</v>
-      </c>
-      <c r="H8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" s="6" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="20">
-        <f>(D5-C5)*24</f>
-        <v>3.5833333333333326</v>
-      </c>
-      <c r="E9" s="20">
-        <f t="shared" ref="E9:O9" si="2">(E5-D5)*24</f>
-        <v>3.2999999999999989</v>
-      </c>
-      <c r="F9" s="20">
-        <f t="shared" si="2"/>
-        <v>2.8166666666666673</v>
-      </c>
-      <c r="G9" s="20">
-        <f t="shared" si="2"/>
-        <v>13.833333333333337</v>
-      </c>
-      <c r="H9" s="20">
-        <f t="shared" si="2"/>
-        <v>-32.583333333333336</v>
-      </c>
-      <c r="I9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N9" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O9" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="8">
-        <f>D8/D9</f>
-        <v>56.677612343124409</v>
-      </c>
-      <c r="E10" s="8">
-        <f t="shared" ref="E10:O10" si="3">E8/E9</f>
-        <v>195.57274876423813</v>
-      </c>
-      <c r="F10" s="8">
-        <f t="shared" si="3"/>
-        <v>102.79445428238247</v>
-      </c>
-      <c r="G10" s="8">
-        <f t="shared" si="3"/>
-        <v>38.921875398935029</v>
-      </c>
-      <c r="H10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O10" s="23" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="13" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B13" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="18">
-        <v>0.37708333333333338</v>
-      </c>
-      <c r="D13" s="17">
-        <v>0.52638888888888891</v>
-      </c>
-      <c r="E13" s="17">
-        <v>0.66388888888888886</v>
-      </c>
-      <c r="F13" s="17">
-        <v>0.78125</v>
-      </c>
-      <c r="G13" s="17">
-        <v>1.3576388888888891</v>
-      </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="19"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
-        <v>4.7</v>
-      </c>
-      <c r="D14" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E14" s="3">
-        <v>4.7</v>
-      </c>
-      <c r="F14" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="G14" s="3">
-        <v>4.8</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5">
-        <f>$C$3*((100/C14)-1)</f>
-        <v>2838.7234042553191</v>
-      </c>
-      <c r="D15" s="9">
-        <f t="shared" ref="D15:O15" si="4">$C$3*((100/D14)-1)</f>
-        <v>2903.4782608695655</v>
-      </c>
-      <c r="E15" s="9">
-        <f t="shared" si="4"/>
-        <v>2838.7234042553191</v>
-      </c>
-      <c r="F15" s="9">
-        <f t="shared" si="4"/>
-        <v>2776.666666666667</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" si="4"/>
-        <v>2776.666666666667</v>
-      </c>
-      <c r="H15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" s="9" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="13" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1">
-        <f>C15-D15</f>
-        <v>-64.754856614246364</v>
-      </c>
-      <c r="E16" s="1">
-        <f>D15-E15</f>
-        <v>64.754856614246364</v>
-      </c>
-      <c r="F16" s="1">
-        <f>E15-F15</f>
-        <v>62.05673758865214</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" ref="G16:O16" si="5">F15-G15</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="1" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="6" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="20">
-        <f>(D13-C13)*24</f>
-        <v>3.5833333333333326</v>
-      </c>
-      <c r="E17" s="20">
-        <f t="shared" ref="E17:O17" si="6">(E13-D13)*24</f>
-        <v>3.2999999999999989</v>
-      </c>
-      <c r="F17" s="20">
-        <f t="shared" si="6"/>
-        <v>2.8166666666666673</v>
-      </c>
-      <c r="G17" s="20">
-        <f t="shared" si="6"/>
-        <v>13.833333333333337</v>
-      </c>
-      <c r="H17" s="20">
-        <f t="shared" si="6"/>
-        <v>-32.583333333333336</v>
-      </c>
-      <c r="I17" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L17" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="22">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="18.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="8">
-        <f>D16/D17</f>
-        <v>-18.071122776068755</v>
-      </c>
-      <c r="E18" s="8">
-        <f t="shared" ref="E18:O18" si="7">E16/E17</f>
-        <v>19.622683822498903</v>
-      </c>
-      <c r="F18" s="8">
-        <f t="shared" si="7"/>
-        <v>22.031977842125016</v>
-      </c>
-      <c r="G18" s="8">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="8" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="8" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="8" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="8" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="8" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="8" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N18" s="8" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="23" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72fe835d-5e95-4512-8ae0-a7b38af25fc8}" enabled="0" method="" siteId="{72fe835d-5e95-4512-8ae0-a7b38af25fc8}" removed="1"/>

</xml_diff>